<commit_message>
Update UL tests for STRIP56 (B2)
</commit_message>
<xml_diff>
--- a/data/corrispondenze_FH_testDC.xlsx
+++ b/data/corrispondenze_FH_testDC.xlsx
@@ -260,8 +260,8 @@
   </sheetPr>
   <dimension ref="A1:XFD56"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0" tabSelected="1">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A23" workbookViewId="0" tabSelected="1">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -17329,7 +17329,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:16384">
+    <row r="38" spans="1:16384" ht="18">
       <c r="A38" s="8" t="inlineStr">
         <is>
           <t>B2</t>
@@ -17341,10 +17341,10 @@
         </is>
       </c>
       <c r="C38" s="2">
-        <v>638</v>
+        <v>914</v>
       </c>
       <c r="D38" s="2">
-        <v>99</v>
+        <v>934</v>
       </c>
     </row>
     <row r="39" spans="1:16384">

</xml_diff>